<commit_message>
refactor(wossal-web): :recycle: add some on upload file and modify the filter
</commit_message>
<xml_diff>
--- a/src/assets/files/template-admin.xlsx
+++ b/src/assets/files/template-admin.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Feuille 1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Template fichier CSV pour impor" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,77 +11,92 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Nom</t>
+  </si>
   <si>
     <t>Prénom</t>
   </si>
   <si>
-    <t>Nom</t>
-  </si>
-  <si>
-    <t>Adresse e-mail</t>
+    <t>Adresse mail</t>
   </si>
   <si>
     <t>Date de naissance</t>
   </si>
   <si>
-    <t>Téléphone</t>
-  </si>
-  <si>
-    <t>Adresse</t>
+    <t>Numéro téléphone</t>
+  </si>
+  <si>
+    <t>Adresse postale</t>
   </si>
   <si>
     <t>Fonction</t>
   </si>
   <si>
-    <t>Identifiant unique</t>
-  </si>
-  <si>
-    <t>salaire</t>
-  </si>
-  <si>
-    <t>Lousa</t>
-  </si>
-  <si>
-    <t>diop</t>
-  </si>
-  <si>
-    <t>loussa@gmail.com</t>
-  </si>
-  <si>
-    <t>addresse1</t>
-  </si>
-  <si>
-    <t>fonction1</t>
+    <t>Matricule</t>
+  </si>
+  <si>
+    <t>Salaire</t>
+  </si>
+  <si>
+    <t>Catégorie socioprofessionnelle</t>
+  </si>
+  <si>
+    <t>DIOP</t>
+  </si>
+  <si>
+    <t>Moussa</t>
+  </si>
+  <si>
+    <t>papemactarndiayepro+testpro@gmail.com</t>
+  </si>
+  <si>
+    <t>Testeur</t>
+  </si>
+  <si>
+    <t>JKSJK892892</t>
+  </si>
+  <si>
+    <t>tests Daly 2003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="dd&quot;-&quot;mm&quot;-&quot;yyyy"/>
-    <numFmt numFmtId="165" formatCode="d-m-yyyy"/>
-    <numFmt numFmtId="166" formatCode="dd-mm-yyyy"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color rgb="FF061E5C"/>
+      <name val="Poppins"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -90,15 +105,16 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="166" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -128,40 +144,40 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4285F4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="EA4335"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="FBBC04"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="34A853"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="FF6D01"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="46BDC6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="1155CC"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="1155CC"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface="Calibri"/>
-        <a:cs typeface="Calibri"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface="Calibri"/>
-        <a:cs typeface="Calibri"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -313,11 +329,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="14.43"/>
-    <col customWidth="1" min="3" max="3" width="47.86"/>
-    <col customWidth="1" min="4" max="6" width="14.43"/>
+    <col customWidth="1" min="1" max="3" width="12.63"/>
+    <col customWidth="1" min="4" max="4" width="25.5"/>
+    <col customWidth="1" min="5" max="5" width="33.0"/>
+    <col customWidth="1" min="6" max="6" width="15.13"/>
+    <col customWidth="1" min="7" max="7" width="24.5"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -333,7 +351,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -348,53 +366,47 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="2">
-        <v>35897.0</v>
+        <v>12</v>
+      </c>
+      <c r="D2" s="3">
+        <v>35417.0</v>
       </c>
       <c r="E2" s="1">
-        <v>2.9029029E8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
+        <f>221784563231</f>
+        <v>221784563231</v>
+      </c>
+      <c r="F2" s="1">
+        <v>9029092.0</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1">
-        <v>1.2892892E7</v>
-      </c>
-      <c r="I2" s="3">
-        <f>1230303</f>
-        <v>1230303</v>
-      </c>
-      <c r="J2" s="3"/>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1">
+        <v>8.2828282E7</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="D3" s="2"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="D4" s="2"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="D6" s="5"/>
-    </row>
+    <row r="3" ht="15.75" customHeight="1"/>
+    <row r="4" ht="15.75" customHeight="1"/>
+    <row r="5" ht="15.75" customHeight="1"/>
+    <row r="6" ht="15.75" customHeight="1"/>
     <row r="7" ht="15.75" customHeight="1"/>
     <row r="8" ht="15.75" customHeight="1"/>
     <row r="9" ht="15.75" customHeight="1"/>

</xml_diff>